<commit_message>
Added the code for extent report Added a testng xml for regression execution
</commit_message>
<xml_diff>
--- a/SeleniumAutomationFWv01/src/main/java/com/crm/qa/testdata/CRMTestInput.xlsx
+++ b/SeleniumAutomationFWv01/src/main/java/com/crm/qa/testdata/CRMTestInput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sayondas/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sayondas/git/SeleniumAutomationFW/SeleniumAutomationFWv01/src/main/java/com/crm/qa/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1A2707B-CDED-004C-983C-B8BCD4070509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E216F84-809D-C54E-AA00-E785E901602B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{B6EDED67-A97A-EC4F-8615-AEBED57B2AEA}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{B6EDED67-A97A-EC4F-8615-AEBED57B2AEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,15 +47,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Sayon</t>
-  </si>
-  <si>
-    <t>Das</t>
-  </si>
-  <si>
-    <t>SDET</t>
-  </si>
-  <si>
     <t>Elkhan</t>
   </si>
   <si>
@@ -63,6 +54,15 @@
   </si>
   <si>
     <t>Automation Tester</t>
+  </si>
+  <si>
+    <t>Konul</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,24 +438,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>